<commit_message>
add Sensitivity, Absorption characteristic and Massbalance
</commit_message>
<xml_diff>
--- a/src/code/templates/WorkflowInput.xlsx
+++ b/src/code/templates/WorkflowInput.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t>reportName</t>
   </si>
@@ -197,13 +197,43 @@
 may be empty</t>
   </si>
   <si>
+    <t>This population is used  in comparison plots as Referencepopulation. Important for workflow type pediatric and ratioComparison. select 1 for true, 0 for false</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>sensXls</t>
+  </si>
+  <si>
+    <t>xlsfilefor sensitivity Parameter definition; if it is empty, sheet is in this xlsfile</t>
+  </si>
+  <si>
+    <t>sensSheet</t>
+  </si>
+  <si>
+    <t>xlssheet for sensitivity Parameter definition; if empty first sheet is taken</t>
+  </si>
+  <si>
+    <t>SensitivityParameter</t>
+  </si>
+  <si>
     <t>Type of the workflow (Only the entry of the first simulation is taken into account). Possible options are 
-- "pediatric" properties (physiology and PK Parameter) are display vs age and weigth
-- "parallelComparison" PK parameter are displayed parrallel in boxwhsiker plots no refernce population
+- "pediatric" properties (physiology and PK Parameter) are display vs age and weigth, sensitivity analysis is done on all populations except reference, first pediatric output defines analysed PK Parameter base
+- "parallelComparison" PK parameter are displayed parrallel in boxwhsiker plots no reference population, sensitivity analysis is done on all populations, first output defines analysed PK Parameter base
 - "ratioComparison" same as parallelComparison, but additional the ratio of the PK Parameter to the reference population is calculated</t>
   </si>
   <si>
-    <t>This population is used  in comparison plots as Referencepopulation. Important for workflow type pediatric and ratioComparison. select 1 for true, 0 for false</t>
+    <t>TaskdoAbsorptionPlots</t>
+  </si>
+  <si>
+    <t>absorption is plotted</t>
+  </si>
+  <si>
+    <t>massbalance will be checked</t>
+  </si>
+  <si>
+    <t>TaskcheckMassbalance</t>
   </si>
 </sst>
 </file>
@@ -624,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -798,42 +828,99 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -843,10 +930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -876,12 +963,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="198" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -954,7 +1041,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1021,7 +1108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>29</v>
       </c>
@@ -1090,70 +1177,105 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add Sensitivity, Absorption characteristic and Massbalance (#11)
add Sensitivity, Absorption characteristic and Massbalance
</commit_message>
<xml_diff>
--- a/src/code/templates/WorkflowInput.xlsx
+++ b/src/code/templates/WorkflowInput.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t>reportName</t>
   </si>
@@ -197,13 +197,43 @@
 may be empty</t>
   </si>
   <si>
+    <t>This population is used  in comparison plots as Referencepopulation. Important for workflow type pediatric and ratioComparison. select 1 for true, 0 for false</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>sensXls</t>
+  </si>
+  <si>
+    <t>xlsfilefor sensitivity Parameter definition; if it is empty, sheet is in this xlsfile</t>
+  </si>
+  <si>
+    <t>sensSheet</t>
+  </si>
+  <si>
+    <t>xlssheet for sensitivity Parameter definition; if empty first sheet is taken</t>
+  </si>
+  <si>
+    <t>SensitivityParameter</t>
+  </si>
+  <si>
     <t>Type of the workflow (Only the entry of the first simulation is taken into account). Possible options are 
-- "pediatric" properties (physiology and PK Parameter) are display vs age and weigth
-- "parallelComparison" PK parameter are displayed parrallel in boxwhsiker plots no refernce population
+- "pediatric" properties (physiology and PK Parameter) are display vs age and weigth, sensitivity analysis is done on all populations except reference, first pediatric output defines analysed PK Parameter base
+- "parallelComparison" PK parameter are displayed parrallel in boxwhsiker plots no reference population, sensitivity analysis is done on all populations, first output defines analysed PK Parameter base
 - "ratioComparison" same as parallelComparison, but additional the ratio of the PK Parameter to the reference population is calculated</t>
   </si>
   <si>
-    <t>This population is used  in comparison plots as Referencepopulation. Important for workflow type pediatric and ratioComparison. select 1 for true, 0 for false</t>
+    <t>TaskdoAbsorptionPlots</t>
+  </si>
+  <si>
+    <t>absorption is plotted</t>
+  </si>
+  <si>
+    <t>massbalance will be checked</t>
+  </si>
+  <si>
+    <t>TaskcheckMassbalance</t>
   </si>
 </sst>
 </file>
@@ -624,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -798,42 +828,99 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -843,10 +930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -876,12 +963,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="198" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -954,7 +1041,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1021,7 +1108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>29</v>
       </c>
@@ -1090,70 +1177,105 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>